<commit_message>
Incorrect handling of subtotals fixed.
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_Simple.xlsx
+++ b/tests/Gauges/GroupTagTests_Simple.xlsx
@@ -8,7 +8,6 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <x:sheet name="__temp_buffer" sheetId="5" state="veryHidden" r:id="rId5"/>
   </x:sheets>
   <x:definedNames>
     <x:definedName name="Orders">Sheet1!$A$12:$J$21</x:definedName>
@@ -392,21 +391,24 @@
     <x:xf numFmtId="0" fontId="13" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="4" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -420,9 +422,6 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="4" fontId="12" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
@@ -647,28 +646,32 @@
       <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -696,10 +699,6 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -1370,236 +1369,236 @@
     </x:row>
     <x:row r="12" spans="1:12" outlineLevel="2">
       <x:c r="A12" s="50" t="s"/>
-      <x:c r="B12" s="78" t="n">
+      <x:c r="B12" s="75" t="n">
         <x:v>1023</x:v>
       </x:c>
-      <x:c r="C12" s="77">
+      <x:c r="C12" s="76">
         <x:v>32325</x:v>
       </x:c>
-      <x:c r="D12" s="77">
+      <x:c r="D12" s="76">
         <x:v>32326</x:v>
       </x:c>
-      <x:c r="E12" s="76" t="s"/>
-      <x:c r="F12" s="76" t="s"/>
-      <x:c r="G12" s="76" t="s">
+      <x:c r="E12" s="77" t="s"/>
+      <x:c r="F12" s="77" t="s"/>
+      <x:c r="G12" s="77" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="H12" s="75" t="n">
+      <x:c r="H12" s="78" t="n">
         <x:v>4674</x:v>
       </x:c>
-      <x:c r="I12" s="75" t="n">
+      <x:c r="I12" s="78" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J12" s="75" t="n">
+      <x:c r="J12" s="78" t="n">
         <x:v>4674</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:12" outlineLevel="2">
       <x:c r="A13" s="50" t="s"/>
-      <x:c r="B13" s="78" t="n">
+      <x:c r="B13" s="75" t="n">
         <x:v>1123</x:v>
       </x:c>
-      <x:c r="C13" s="77">
+      <x:c r="C13" s="76">
         <x:v>34205</x:v>
       </x:c>
-      <x:c r="D13" s="77">
+      <x:c r="D13" s="76">
         <x:v>34205</x:v>
       </x:c>
-      <x:c r="E13" s="76" t="s"/>
-      <x:c r="F13" s="76" t="s"/>
-      <x:c r="G13" s="76" t="s">
+      <x:c r="E13" s="77" t="s"/>
+      <x:c r="F13" s="77" t="s"/>
+      <x:c r="G13" s="77" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="H13" s="75" t="n">
+      <x:c r="H13" s="78" t="n">
         <x:v>13945</x:v>
       </x:c>
-      <x:c r="I13" s="75" t="n">
+      <x:c r="I13" s="78" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J13" s="75" t="n">
+      <x:c r="J13" s="78" t="n">
         <x:v>13945</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:12" outlineLevel="1">
       <x:c r="A14" s="50" t="s"/>
-      <x:c r="B14" s="81" t="n"/>
-      <x:c r="C14" s="82" t="s"/>
-      <x:c r="D14" s="83" t="s"/>
-      <x:c r="E14" s="82" t="s"/>
-      <x:c r="F14" s="84" t="s"/>
-      <x:c r="G14" s="85" t="s">
+      <x:c r="B14" s="82" t="s"/>
+      <x:c r="C14" s="83" t="s"/>
+      <x:c r="D14" s="84" t="s"/>
+      <x:c r="E14" s="83" t="s"/>
+      <x:c r="F14" s="85" t="s"/>
+      <x:c r="G14" s="86" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="H14" s="86">
+      <x:c r="H14" s="87">
         <x:f>Subtotal(9,H12:H13)</x:f>
       </x:c>
-      <x:c r="I14" s="87" t="n"/>
-      <x:c r="J14" s="86">
+      <x:c r="I14" s="88" t="s"/>
+      <x:c r="J14" s="87">
         <x:f>Subtotal(9,J12:J13)</x:f>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:12" outlineLevel="2">
       <x:c r="A15" s="50" t="s"/>
-      <x:c r="B15" s="78" t="n">
+      <x:c r="B15" s="75" t="n">
         <x:v>1269</x:v>
       </x:c>
-      <x:c r="C15" s="77">
+      <x:c r="C15" s="76">
         <x:v>34684</x:v>
       </x:c>
-      <x:c r="D15" s="77">
+      <x:c r="D15" s="76">
         <x:v>34684</x:v>
       </x:c>
-      <x:c r="E15" s="76" t="s"/>
-      <x:c r="F15" s="76" t="s"/>
-      <x:c r="G15" s="76" t="s">
+      <x:c r="E15" s="77" t="s"/>
+      <x:c r="F15" s="77" t="s"/>
+      <x:c r="G15" s="77" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="H15" s="75" t="n">
+      <x:c r="H15" s="78" t="n">
         <x:v>1400</x:v>
       </x:c>
-      <x:c r="I15" s="75" t="n">
+      <x:c r="I15" s="78" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J15" s="75" t="n">
+      <x:c r="J15" s="78" t="n">
         <x:v>1400</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:12" customFormat="1" ht="12" customHeight="1" outlineLevel="2">
       <x:c r="A16" s="50" t="s"/>
-      <x:c r="B16" s="78" t="n">
+      <x:c r="B16" s="75" t="n">
         <x:v>1169</x:v>
       </x:c>
-      <x:c r="C16" s="77">
+      <x:c r="C16" s="76">
         <x:v>34521</x:v>
       </x:c>
-      <x:c r="D16" s="77">
+      <x:c r="D16" s="76">
         <x:v>34521</x:v>
       </x:c>
-      <x:c r="E16" s="76" t="s"/>
-      <x:c r="F16" s="76" t="s"/>
-      <x:c r="G16" s="76" t="s">
+      <x:c r="E16" s="77" t="s"/>
+      <x:c r="F16" s="77" t="s"/>
+      <x:c r="G16" s="77" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="H16" s="75" t="n">
+      <x:c r="H16" s="78" t="n">
         <x:v>9471.95</x:v>
       </x:c>
-      <x:c r="I16" s="75" t="n">
+      <x:c r="I16" s="78" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J16" s="75" t="n">
+      <x:c r="J16" s="78" t="n">
         <x:v>9471.95</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:12" outlineLevel="1">
       <x:c r="A17" s="50" t="s"/>
-      <x:c r="B17" s="81" t="n"/>
-      <x:c r="C17" s="82" t="s"/>
-      <x:c r="D17" s="83" t="s"/>
-      <x:c r="E17" s="82" t="s"/>
-      <x:c r="F17" s="84" t="s"/>
-      <x:c r="G17" s="85" t="s">
+      <x:c r="B17" s="82" t="s"/>
+      <x:c r="C17" s="83" t="s"/>
+      <x:c r="D17" s="84" t="s"/>
+      <x:c r="E17" s="83" t="s"/>
+      <x:c r="F17" s="85" t="s"/>
+      <x:c r="G17" s="86" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="H17" s="86">
+      <x:c r="H17" s="87">
         <x:f>Subtotal(9,H15:H16)</x:f>
       </x:c>
-      <x:c r="I17" s="87" t="n"/>
-      <x:c r="J17" s="86">
+      <x:c r="I17" s="88" t="s"/>
+      <x:c r="J17" s="87">
         <x:f>Subtotal(9,J15:J16)</x:f>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:12" outlineLevel="2">
       <x:c r="A18" s="50" t="s"/>
-      <x:c r="B18" s="78" t="n">
+      <x:c r="B18" s="75" t="n">
         <x:v>1176</x:v>
       </x:c>
-      <x:c r="C18" s="77">
+      <x:c r="C18" s="76">
         <x:v>34541</x:v>
       </x:c>
-      <x:c r="D18" s="77">
+      <x:c r="D18" s="76">
         <x:v>34541</x:v>
       </x:c>
-      <x:c r="E18" s="76" t="s"/>
-      <x:c r="F18" s="76" t="s"/>
-      <x:c r="G18" s="76" t="s">
+      <x:c r="E18" s="77" t="s"/>
+      <x:c r="F18" s="77" t="s"/>
+      <x:c r="G18" s="77" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="H18" s="75" t="n">
+      <x:c r="H18" s="78" t="n">
         <x:v>4178.85</x:v>
       </x:c>
-      <x:c r="I18" s="75" t="n">
+      <x:c r="I18" s="78" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J18" s="75" t="n">
+      <x:c r="J18" s="78" t="n">
         <x:v>4178.85</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:12" outlineLevel="2">
       <x:c r="A19" s="50" t="s"/>
-      <x:c r="B19" s="78" t="n">
+      <x:c r="B19" s="75" t="n">
         <x:v>1076</x:v>
       </x:c>
-      <x:c r="C19" s="77">
+      <x:c r="C19" s="76">
         <x:v>34684</x:v>
       </x:c>
-      <x:c r="D19" s="77">
+      <x:c r="D19" s="76">
         <x:v>32624</x:v>
       </x:c>
-      <x:c r="E19" s="76" t="s"/>
-      <x:c r="F19" s="76" t="s"/>
-      <x:c r="G19" s="76" t="s">
+      <x:c r="E19" s="77" t="s"/>
+      <x:c r="F19" s="77" t="s"/>
+      <x:c r="G19" s="77" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="H19" s="75" t="n">
+      <x:c r="H19" s="78" t="n">
         <x:v>17781</x:v>
       </x:c>
-      <x:c r="I19" s="75" t="n">
+      <x:c r="I19" s="78" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J19" s="75" t="n">
+      <x:c r="J19" s="78" t="n">
         <x:v>17781</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:12" outlineLevel="1">
       <x:c r="A20" s="50" t="s"/>
-      <x:c r="B20" s="81" t="s"/>
-      <x:c r="C20" s="82" t="s"/>
-      <x:c r="D20" s="83" t="s"/>
-      <x:c r="E20" s="82" t="s"/>
-      <x:c r="F20" s="84" t="s"/>
-      <x:c r="G20" s="85" t="s">
+      <x:c r="B20" s="82" t="s"/>
+      <x:c r="C20" s="83" t="s"/>
+      <x:c r="D20" s="84" t="s"/>
+      <x:c r="E20" s="83" t="s"/>
+      <x:c r="F20" s="85" t="s"/>
+      <x:c r="G20" s="86" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="H20" s="86">
+      <x:c r="H20" s="87">
         <x:f>Subtotal(9,H18:H19)</x:f>
       </x:c>
-      <x:c r="I20" s="87" t="s"/>
-      <x:c r="J20" s="86">
+      <x:c r="I20" s="88" t="s"/>
+      <x:c r="J20" s="87">
         <x:f>Subtotal(9,J18:J19)</x:f>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:12">
       <x:c r="A21" s="50" t="s"/>
-      <x:c r="B21" s="81" t="s">
+      <x:c r="B21" s="82" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="C21" s="82" t="s"/>
-      <x:c r="D21" s="83" t="s"/>
-      <x:c r="E21" s="82" t="s"/>
-      <x:c r="F21" s="84" t="s"/>
-      <x:c r="G21" s="85" t="s"/>
-      <x:c r="H21" s="86">
+      <x:c r="C21" s="83" t="s"/>
+      <x:c r="D21" s="84" t="s"/>
+      <x:c r="E21" s="83" t="s"/>
+      <x:c r="F21" s="85" t="s"/>
+      <x:c r="G21" s="86" t="s"/>
+      <x:c r="H21" s="87">
         <x:f>Subtotal(9,H12:H19)</x:f>
       </x:c>
-      <x:c r="I21" s="87" t="s"/>
-      <x:c r="J21" s="86">
+      <x:c r="I21" s="88" t="s"/>
+      <x:c r="J21" s="87">
         <x:f>Subtotal(9,J12:J19)</x:f>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:12">
       <x:c r="A22" s="50" t="s"/>
       <x:c r="B22" s="50" t="s"/>
-      <x:c r="C22" s="88" t="s"/>
+      <x:c r="C22" s="81" t="s"/>
       <x:c r="D22" s="50" t="s"/>
       <x:c r="E22" s="50" t="s"/>
       <x:c r="F22" s="50" t="s"/>
@@ -1619,15 +1618,15 @@
     </x:row>
     <x:row r="24" spans="1:12">
       <x:c r="A24" s="50" t="s"/>
-      <x:c r="B24" s="79" t="s">
+      <x:c r="B24" s="80" t="s">
         <x:v>30</x:v>
       </x:c>
       <x:c r="C24" s="62" t="s"/>
       <x:c r="D24" s="62" t="s"/>
-      <x:c r="E24" s="79" t="s">
+      <x:c r="E24" s="80" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="F24" s="80" t="s"/>
+      <x:c r="F24" s="79" t="s"/>
     </x:row>
     <x:row r="25" spans="1:12">
       <x:c r="G25" s="50" t="s"/>
@@ -1673,202 +1672,4 @@
   <x:drawing r:id="rId2"/>
   <x:tableParts count="0"/>
 </x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:J7"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:10">
-      <x:c r="A1" s="50" t="s"/>
-      <x:c r="B1" s="78" t="n">
-        <x:v>1023</x:v>
-      </x:c>
-      <x:c r="C1" s="77">
-        <x:v>32325</x:v>
-      </x:c>
-      <x:c r="D1" s="77">
-        <x:v>32326</x:v>
-      </x:c>
-      <x:c r="E1" s="76" t="s"/>
-      <x:c r="F1" s="76" t="s"/>
-      <x:c r="G1" s="76" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="H1" s="75" t="n">
-        <x:v>4674</x:v>
-      </x:c>
-      <x:c r="I1" s="75" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J1" s="75" t="n">
-        <x:v>4674</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:10">
-      <x:c r="A2" s="50" t="s"/>
-      <x:c r="B2" s="78" t="n">
-        <x:v>1076</x:v>
-      </x:c>
-      <x:c r="C2" s="77">
-        <x:v>34684</x:v>
-      </x:c>
-      <x:c r="D2" s="77">
-        <x:v>32624</x:v>
-      </x:c>
-      <x:c r="E2" s="76" t="s"/>
-      <x:c r="F2" s="76" t="s"/>
-      <x:c r="G2" s="76" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="H2" s="75" t="n">
-        <x:v>17781</x:v>
-      </x:c>
-      <x:c r="I2" s="75" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J2" s="75" t="n">
-        <x:v>17781</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:10">
-      <x:c r="A3" s="50" t="s"/>
-      <x:c r="B3" s="78" t="n">
-        <x:v>1123</x:v>
-      </x:c>
-      <x:c r="C3" s="77">
-        <x:v>34205</x:v>
-      </x:c>
-      <x:c r="D3" s="77">
-        <x:v>34205</x:v>
-      </x:c>
-      <x:c r="E3" s="76" t="s"/>
-      <x:c r="F3" s="76" t="s"/>
-      <x:c r="G3" s="76" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="H3" s="75" t="n">
-        <x:v>13945</x:v>
-      </x:c>
-      <x:c r="I3" s="75" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J3" s="75" t="n">
-        <x:v>13945</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:10">
-      <x:c r="A4" s="50" t="s"/>
-      <x:c r="B4" s="78" t="n">
-        <x:v>1169</x:v>
-      </x:c>
-      <x:c r="C4" s="77">
-        <x:v>34521</x:v>
-      </x:c>
-      <x:c r="D4" s="77">
-        <x:v>34521</x:v>
-      </x:c>
-      <x:c r="E4" s="76" t="s"/>
-      <x:c r="F4" s="76" t="s"/>
-      <x:c r="G4" s="76" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="H4" s="75" t="n">
-        <x:v>9471.95</x:v>
-      </x:c>
-      <x:c r="I4" s="75" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J4" s="75" t="n">
-        <x:v>9471.95</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:10">
-      <x:c r="A5" s="50" t="s"/>
-      <x:c r="B5" s="78" t="n">
-        <x:v>1176</x:v>
-      </x:c>
-      <x:c r="C5" s="77">
-        <x:v>34541</x:v>
-      </x:c>
-      <x:c r="D5" s="77">
-        <x:v>34541</x:v>
-      </x:c>
-      <x:c r="E5" s="76" t="s"/>
-      <x:c r="F5" s="76" t="s"/>
-      <x:c r="G5" s="76" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="H5" s="75" t="n">
-        <x:v>4178.85</x:v>
-      </x:c>
-      <x:c r="I5" s="75" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J5" s="75" t="n">
-        <x:v>4178.85</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:10">
-      <x:c r="A6" s="50" t="s"/>
-      <x:c r="B6" s="78" t="n">
-        <x:v>1269</x:v>
-      </x:c>
-      <x:c r="C6" s="77">
-        <x:v>34684</x:v>
-      </x:c>
-      <x:c r="D6" s="77">
-        <x:v>34684</x:v>
-      </x:c>
-      <x:c r="E6" s="76" t="s"/>
-      <x:c r="F6" s="76" t="s"/>
-      <x:c r="G6" s="76" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="H6" s="75" t="n">
-        <x:v>1400</x:v>
-      </x:c>
-      <x:c r="I6" s="75" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J6" s="75" t="n">
-        <x:v>1400</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:10">
-      <x:c r="A7" s="50" t="s"/>
-      <x:c r="B7" s="81" t="s"/>
-      <x:c r="C7" s="82" t="s"/>
-      <x:c r="D7" s="83" t="s"/>
-      <x:c r="E7" s="82" t="s"/>
-      <x:c r="F7" s="84" t="s"/>
-      <x:c r="G7" s="85" t="s"/>
-      <x:c r="H7" s="86" t="s"/>
-      <x:c r="I7" s="87" t="s"/>
-      <x:c r="J7" s="86" t="s"/>
-    </x:row>
-  </x:sheetData>
-  <x:conditionalFormatting sqref="B1:B6">
-    <x:cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
-      <x:formula>$G1="Visa"</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="E1:G6">
-    <x:cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
-      <x:formula>$G1="Visa"</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
 </file>
</xml_diff>